<commit_message>
Agrupamento com GROUP BY
</commit_message>
<xml_diff>
--- a/agrupamento/Agrupamento - Tabela exemplo.xlsx
+++ b/agrupamento/Agrupamento - Tabela exemplo.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Função de Agregação" sheetId="1" r:id="rId1"/>
+    <sheet name="Agrupamento" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="104">
   <si>
     <t>Exemplo para agrupamento</t>
   </si>
@@ -161,9 +162,6 @@
     <t>select cpf from pessoa</t>
   </si>
   <si>
-    <t>funções de agregação</t>
-  </si>
-  <si>
     <t>count()</t>
   </si>
   <si>
@@ -246,13 +244,113 @@
   </si>
   <si>
     <t>select sum(peso) as pesoTotal from pessoa;</t>
+  </si>
+  <si>
+    <t>Funções de agregação</t>
+  </si>
+  <si>
+    <t>select count(cpf) as quantidadeDePessoas from pessoa where idade &gt;= 18;</t>
+  </si>
+  <si>
+    <t>Fazendo filtros usando o WHERE: o filtro é feito antes de agregar</t>
+  </si>
+  <si>
+    <t>select avg(idade) as mediaDeIdade from pessoa where sexo = 'F';</t>
+  </si>
+  <si>
+    <t>select count(cpf) as quantidadeDePessoas, avg(idade) mediaDeIdade from pessoa where estado = 'MG';</t>
+  </si>
+  <si>
+    <t>select count(cpf) as quantidadeDePessoas, min(peso) as maisLeve, max(idade) as maisVelho from pessoa where ativo = true;</t>
+  </si>
+  <si>
+    <t>Preparação:</t>
+  </si>
+  <si>
+    <t>Consultar todos os estados:</t>
+  </si>
+  <si>
+    <t>select estado from pessoa;</t>
+  </si>
+  <si>
+    <t>Pergunta: quantas pessoas moram em cada estado?</t>
+  </si>
+  <si>
+    <t>Tentativas</t>
+  </si>
+  <si>
+    <t>select count(cpf) as quantidadeDePessoas from pessoa where estado = 'RJ';</t>
+  </si>
+  <si>
+    <t>GROUP BY</t>
+  </si>
+  <si>
+    <t>- normalmente é usado em conjunto com as funções de agregação</t>
+  </si>
+  <si>
+    <t>- agrupa os resultados de uma consulta</t>
+  </si>
+  <si>
+    <t>Sintax:</t>
+  </si>
+  <si>
+    <t>Resposta</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>SELECT campo1, função_de_agregação(campo2) as alias_do_campo
+FROM tabela
+WHERE filtro --filtra antes de agrupar
+GROUP BY campo1
+ORDER BY campo1</t>
+  </si>
+  <si>
+    <t>SELECT estado, count(cpf) as quantidade FROM pessoa GROUP BY estado ORDER by quantidade;</t>
+  </si>
+  <si>
+    <t>Outro exemplo:</t>
+  </si>
+  <si>
+    <t>SELECT estado, count(cpf) as quantidade, min(idade) maisNovo FROM pessoa GROUP BY estado ORDER by estado;</t>
+  </si>
+  <si>
+    <t>Agrupando por mais campos, basta separar os campos por vírgula</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - normalmente os campos utilizados no GROUP BY, são também mostrados no SELECT</t>
+  </si>
+  <si>
+    <t>Regra dos campos</t>
+  </si>
+  <si>
+    <t>Todos os campos que aparecem no SELECT e não pertencem a nenhuma função de agregação, devem aparecer no GROUP BY</t>
+  </si>
+  <si>
+    <t>Cuidado:</t>
+  </si>
+  <si>
+    <t>SELECT estado, count(cidade) qtdCidade, count(cpf) as quantidade
+FROM pessoa
+GROUP BY estado
+ORDER by estado;</t>
+  </si>
+  <si>
+    <t>Consulta cuidado:</t>
+  </si>
+  <si>
+    <t>qtdCidade</t>
+  </si>
+  <si>
+    <t>quantidade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,16 +366,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -300,11 +419,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -313,6 +441,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +859,7 @@
         <v>14</v>
       </c>
       <c r="K6" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -742,10 +888,10 @@
         <v>19</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L7" t="s">
         <v>50</v>
-      </c>
-      <c r="L7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -774,10 +920,10 @@
         <v>14</v>
       </c>
       <c r="K8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -806,10 +952,10 @@
         <v>14</v>
       </c>
       <c r="K9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
@@ -838,7 +984,7 @@
         <v>14</v>
       </c>
       <c r="L10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -893,10 +1039,10 @@
         <v>14</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -925,10 +1071,10 @@
         <v>19</v>
       </c>
       <c r="K13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
@@ -983,10 +1129,10 @@
         <v>14</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -1015,10 +1161,10 @@
         <v>14</v>
       </c>
       <c r="K16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1073,10 +1219,10 @@
         <v>14</v>
       </c>
       <c r="K18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L18" t="s">
         <v>61</v>
-      </c>
-      <c r="L18" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1105,10 +1251,10 @@
         <v>14</v>
       </c>
       <c r="K19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1162,11 +1308,11 @@
       <c r="I21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K21" t="s">
-        <v>67</v>
+      <c r="K21" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="L21" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1194,8 +1340,11 @@
       <c r="I22" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="K22" t="s">
+        <v>52</v>
+      </c>
       <c r="L22" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1226,7 +1375,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1">
         <f>COUNTA(B5:B23)</f>
@@ -1260,16 +1409,16 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>70</v>
+      <c r="K24" t="s">
+        <v>66</v>
       </c>
       <c r="L24" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1282,16 +1431,13 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="K25" t="s">
-        <v>53</v>
-      </c>
       <c r="L25" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1307,7 +1453,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1320,10 +1466,13 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
+      <c r="K27" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1336,6 +1485,38 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>6</v>
+      </c>
+      <c r="L30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>7</v>
+      </c>
+      <c r="L31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1345,4 +1526,746 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N35"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" customWidth="1"/>
+    <col min="13" max="13" width="64.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="8">
+        <v>30</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="8">
+        <v>50</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="16">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="8">
+        <v>22</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="8">
+        <v>55</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>80</v>
+      </c>
+      <c r="N6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
+        <v>8</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8">
+        <v>17</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="8">
+        <v>60</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
+        <v>10</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="8">
+        <v>25</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="8">
+        <v>65</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="16">
+        <v>14</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="8">
+        <v>20</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="8">
+        <v>70</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="16">
+        <v>18</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="8">
+        <v>41</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="8">
+        <v>75</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="16">
+        <v>16</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="8">
+        <v>40</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="8">
+        <v>50</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="16">
+        <v>17</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="8">
+        <v>40</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="8">
+        <v>55</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" t="s">
+        <v>85</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="16">
+        <v>1</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="8">
+        <v>20</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="8">
+        <v>60</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="16">
+        <v>4</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="8">
+        <v>35</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="8">
+        <v>65</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="16">
+        <v>7</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="8">
+        <v>26</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="8">
+        <v>70</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16">
+        <v>11</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="8">
+        <v>30</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="8">
+        <v>75</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="16">
+        <v>2</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="8">
+        <v>30</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="8">
+        <v>50</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="12"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="16">
+        <v>6</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="8">
+        <v>40</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="8">
+        <v>55</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="12"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="16">
+        <v>12</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="8">
+        <v>15</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="8">
+        <v>60</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19" s="12"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="16">
+        <v>5</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="8">
+        <v>13</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="8">
+        <v>65</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" s="12"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="16">
+        <v>9</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="8">
+        <v>28</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="8">
+        <v>70</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="16">
+        <v>13</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="8">
+        <v>27</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="8">
+        <v>75</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" t="s">
+        <v>89</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="16">
+        <v>19</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="8">
+        <v>27</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="8">
+        <v>50</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M23" s="11"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>93</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="K26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="3">
+        <v>3</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="3">
+        <v>3</v>
+      </c>
+      <c r="G27" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="3">
+        <v>10</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="3">
+        <v>10</v>
+      </c>
+      <c r="G28" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="3">
+        <v>6</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="3">
+        <v>6</v>
+      </c>
+      <c r="G29" s="3">
+        <v>6</v>
+      </c>
+      <c r="K29" t="s">
+        <v>97</v>
+      </c>
+      <c r="M29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="M30" s="6"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>99</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M33" s="12"/>
+    </row>
+    <row r="34" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M34" s="12"/>
+    </row>
+    <row r="35" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M35" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="M16:M20"/>
+    <mergeCell ref="M32:M35"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>